<commit_message>
Add types map in pb_build_in_typs.py Add some content to parse table.
</commit_message>
<xml_diff>
--- a/table-builder/builder/table-builder-test/log packet struction.xlsx
+++ b/table-builder/builder/table-builder-test/log packet struction.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,6 +151,10 @@
   </si>
   <si>
     <t>column description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -525,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -537,12 +541,15 @@
     <col min="2" max="2" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
build successfully excel table pb message.
</commit_message>
<xml_diff>
--- a/table-builder/builder/table-builder-test/log packet struction.xlsx
+++ b/table-builder/builder/table-builder-test/log packet struction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="table attribute" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,10 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>char[]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,10 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>char[]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">key name for code </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -86,10 +78,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>char[]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">key type for code </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -155,6 +143,10 @@
   </si>
   <si>
     <t>table description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -531,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -543,10 +535,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -564,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -580,10 +572,10 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -591,39 +583,39 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -661,10 +653,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -678,10 +670,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -695,41 +687,41 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>